<commit_message>
[新規] sub_detectionコマンドを追加 fixed #375
Signed-off-by: nkodama <kodama.naoki@gmail.com>
</commit_message>
<xml_diff>
--- a/HoI2Editor/Documents/Design/commands.xlsx
+++ b/HoI2Editor/Documents/Design/commands.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="989">
   <si>
     <t>trigger</t>
     <phoneticPr fontId="1"/>
@@ -3942,6 +3942,18 @@
   </si>
   <si>
     <t>Stockpile</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sub_detection</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SubDetection</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>string</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4288,11 +4300,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H282"/>
+  <dimension ref="A1:H283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B271" sqref="B271"/>
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A228" sqref="A228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7463,44 +7475,47 @@
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A228" t="s">
-        <v>479</v>
+        <v>986</v>
       </c>
       <c r="B228" t="s">
-        <v>480</v>
+        <v>987</v>
       </c>
       <c r="C228" t="s">
-        <v>481</v>
+        <v>10</v>
       </c>
       <c r="D228" t="s">
-        <v>979</v>
+        <v>211</v>
+      </c>
+      <c r="E228" t="s">
+        <v>988</v>
       </c>
       <c r="G228" t="s">
-        <v>789</v>
+        <v>478</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A229" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B229" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C229" t="s">
         <v>481</v>
       </c>
       <c r="D229" t="s">
-        <v>484</v>
+        <v>979</v>
       </c>
       <c r="G229" t="s">
-        <v>487</v>
+        <v>789</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A230" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B230" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C230" t="s">
         <v>481</v>
@@ -7514,16 +7529,16 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A231" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B231" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C231" t="s">
         <v>481</v>
       </c>
-      <c r="F231" t="s">
-        <v>642</v>
+      <c r="D231" t="s">
+        <v>484</v>
       </c>
       <c r="G231" t="s">
         <v>487</v>
@@ -7531,16 +7546,16 @@
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A232" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B232" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C232" t="s">
-        <v>492</v>
-      </c>
-      <c r="D232" t="s">
-        <v>979</v>
+        <v>481</v>
+      </c>
+      <c r="F232" t="s">
+        <v>642</v>
       </c>
       <c r="G232" t="s">
         <v>487</v>
@@ -7548,10 +7563,10 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A233" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B233" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C233" t="s">
         <v>492</v>
@@ -7565,16 +7580,16 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A234" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B234" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C234" t="s">
         <v>492</v>
       </c>
       <c r="D234" t="s">
-        <v>497</v>
+        <v>979</v>
       </c>
       <c r="G234" t="s">
         <v>487</v>
@@ -7582,10 +7597,10 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A235" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B235" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C235" t="s">
         <v>492</v>
@@ -7599,16 +7614,16 @@
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A236" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B236" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C236" t="s">
         <v>492</v>
       </c>
-      <c r="F236" t="s">
-        <v>642</v>
+      <c r="D236" t="s">
+        <v>497</v>
       </c>
       <c r="G236" t="s">
         <v>487</v>
@@ -7616,19 +7631,16 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A237" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B237" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C237" t="s">
-        <v>121</v>
-      </c>
-      <c r="D237" t="s">
-        <v>215</v>
+        <v>492</v>
       </c>
       <c r="F237" t="s">
-        <v>10</v>
+        <v>642</v>
       </c>
       <c r="G237" t="s">
         <v>487</v>
@@ -7636,16 +7648,19 @@
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A238" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B238" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C238" t="s">
         <v>121</v>
       </c>
       <c r="D238" t="s">
-        <v>642</v>
+        <v>215</v>
+      </c>
+      <c r="F238" t="s">
+        <v>10</v>
       </c>
       <c r="G238" t="s">
         <v>487</v>
@@ -7653,16 +7668,16 @@
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A239" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B239" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C239" t="s">
-        <v>214</v>
+        <v>121</v>
       </c>
       <c r="D239" t="s">
-        <v>215</v>
+        <v>642</v>
       </c>
       <c r="G239" t="s">
         <v>487</v>
@@ -7670,10 +7685,10 @@
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A240" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B240" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C240" t="s">
         <v>214</v>
@@ -7687,16 +7702,16 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A241" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B241" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C241" t="s">
-        <v>121</v>
+        <v>214</v>
       </c>
       <c r="D241" t="s">
-        <v>979</v>
+        <v>215</v>
       </c>
       <c r="G241" t="s">
         <v>487</v>
@@ -7704,10 +7719,10 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A242" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B242" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C242" t="s">
         <v>121</v>
@@ -7721,13 +7736,13 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A243" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B243" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C243" t="s">
-        <v>481</v>
+        <v>121</v>
       </c>
       <c r="D243" t="s">
         <v>979</v>
@@ -7738,10 +7753,10 @@
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A244" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B244" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C244" t="s">
         <v>481</v>
@@ -7755,10 +7770,13 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A245" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B245" t="s">
-        <v>522</v>
+        <v>520</v>
+      </c>
+      <c r="C245" t="s">
+        <v>481</v>
       </c>
       <c r="D245" t="s">
         <v>979</v>
@@ -7769,10 +7787,10 @@
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A246" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B246" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D246" t="s">
         <v>979</v>
@@ -7783,13 +7801,13 @@
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A247" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B247" t="s">
-        <v>526</v>
-      </c>
-      <c r="C247" t="s">
-        <v>642</v>
+        <v>524</v>
+      </c>
+      <c r="D247" t="s">
+        <v>979</v>
       </c>
       <c r="G247" t="s">
         <v>487</v>
@@ -7797,10 +7815,10 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A248" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B248" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C248" t="s">
         <v>642</v>
@@ -7811,47 +7829,41 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A249" t="s">
-        <v>505</v>
+        <v>527</v>
       </c>
       <c r="B249" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C249" t="s">
-        <v>170</v>
-      </c>
-      <c r="D249" t="s">
-        <v>215</v>
+        <v>642</v>
       </c>
       <c r="G249" t="s">
-        <v>502</v>
+        <v>487</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A250" t="s">
-        <v>530</v>
+        <v>505</v>
       </c>
       <c r="B250" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C250" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
       <c r="D250" t="s">
         <v>215</v>
       </c>
-      <c r="F250" t="s">
-        <v>10</v>
-      </c>
       <c r="G250" t="s">
-        <v>536</v>
+        <v>502</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A251" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B251" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C251" t="s">
         <v>121</v>
@@ -7868,10 +7880,10 @@
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A252" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B252" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C252" t="s">
         <v>121</v>
@@ -7888,10 +7900,10 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A253" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="B253" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="C253" t="s">
         <v>121</v>
@@ -7908,47 +7920,53 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A254" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="B254" t="s">
-        <v>545</v>
+        <v>541</v>
+      </c>
+      <c r="C254" t="s">
+        <v>121</v>
       </c>
       <c r="D254" t="s">
         <v>215</v>
       </c>
+      <c r="F254" t="s">
+        <v>10</v>
+      </c>
       <c r="G254" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A255" t="s">
-        <v>909</v>
+        <v>546</v>
       </c>
       <c r="B255" t="s">
-        <v>957</v>
-      </c>
-      <c r="C255" t="s">
-        <v>979</v>
-      </c>
-      <c r="E255" t="s">
-        <v>979</v>
-      </c>
-      <c r="F255" t="s">
-        <v>642</v>
+        <v>545</v>
+      </c>
+      <c r="D255" t="s">
+        <v>215</v>
       </c>
       <c r="G255" t="s">
-        <v>912</v>
+        <v>536</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A256" t="s">
-        <v>940</v>
+        <v>909</v>
       </c>
       <c r="B256" t="s">
-        <v>913</v>
+        <v>957</v>
       </c>
       <c r="C256" t="s">
         <v>979</v>
+      </c>
+      <c r="E256" t="s">
+        <v>979</v>
+      </c>
+      <c r="F256" t="s">
+        <v>642</v>
       </c>
       <c r="G256" t="s">
         <v>912</v>
@@ -7956,16 +7974,13 @@
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A257" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B257" t="s">
-        <v>958</v>
+        <v>913</v>
       </c>
       <c r="C257" t="s">
-        <v>914</v>
-      </c>
-      <c r="F257" t="s">
-        <v>642</v>
+        <v>979</v>
       </c>
       <c r="G257" t="s">
         <v>912</v>
@@ -7973,13 +7988,13 @@
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A258" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B258" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="C258" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="F258" t="s">
         <v>642</v>
@@ -7990,30 +8005,36 @@
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A259" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B259" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C259" t="s">
-        <v>916</v>
-      </c>
-      <c r="D259" t="s">
-        <v>979</v>
-      </c>
-      <c r="E259" t="s">
-        <v>917</v>
+        <v>915</v>
+      </c>
+      <c r="F259" t="s">
+        <v>642</v>
       </c>
       <c r="G259" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A260" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B260" t="s">
-        <v>918</v>
+        <v>960</v>
+      </c>
+      <c r="C260" t="s">
+        <v>916</v>
+      </c>
+      <c r="D260" t="s">
+        <v>979</v>
+      </c>
+      <c r="E260" t="s">
+        <v>917</v>
       </c>
       <c r="G260" t="s">
         <v>920</v>
@@ -8021,55 +8042,49 @@
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A261" t="s">
-        <v>919</v>
+        <v>944</v>
       </c>
       <c r="B261" t="s">
-        <v>961</v>
-      </c>
-      <c r="C261" t="s">
-        <v>642</v>
-      </c>
-      <c r="D261" t="s">
-        <v>979</v>
-      </c>
-      <c r="E261" t="s">
-        <v>979</v>
-      </c>
-      <c r="F261" t="s">
-        <v>642</v>
+        <v>918</v>
       </c>
       <c r="G261" t="s">
         <v>920</v>
       </c>
-      <c r="H261" t="s">
-        <v>921</v>
-      </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A262" t="s">
-        <v>945</v>
+        <v>919</v>
       </c>
       <c r="B262" t="s">
-        <v>962</v>
+        <v>961</v>
+      </c>
+      <c r="C262" t="s">
+        <v>642</v>
       </c>
       <c r="D262" t="s">
         <v>979</v>
+      </c>
+      <c r="E262" t="s">
+        <v>979</v>
+      </c>
+      <c r="F262" t="s">
+        <v>642</v>
       </c>
       <c r="G262" t="s">
         <v>920</v>
       </c>
+      <c r="H262" t="s">
+        <v>921</v>
+      </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A263" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B263" t="s">
-        <v>963</v>
-      </c>
-      <c r="C263" t="s">
-        <v>642</v>
-      </c>
-      <c r="F263" t="s">
+        <v>962</v>
+      </c>
+      <c r="D263" t="s">
         <v>979</v>
       </c>
       <c r="G263" t="s">
@@ -8078,13 +8093,13 @@
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A264" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B264" t="s">
-        <v>923</v>
+        <v>963</v>
       </c>
       <c r="C264" t="s">
-        <v>914</v>
+        <v>642</v>
       </c>
       <c r="F264" t="s">
         <v>979</v>
@@ -8095,19 +8110,16 @@
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A265" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B265" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C265" t="s">
-        <v>642</v>
-      </c>
-      <c r="D265" t="s">
-        <v>979</v>
+        <v>914</v>
       </c>
       <c r="F265" t="s">
-        <v>642</v>
+        <v>979</v>
       </c>
       <c r="G265" t="s">
         <v>920</v>
@@ -8115,10 +8127,10 @@
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A266" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B266" t="s">
-        <v>964</v>
+        <v>924</v>
       </c>
       <c r="C266" t="s">
         <v>642</v>
@@ -8135,30 +8147,30 @@
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A267" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B267" t="s">
-        <v>925</v>
+        <v>964</v>
       </c>
       <c r="C267" t="s">
         <v>642</v>
       </c>
       <c r="D267" t="s">
-        <v>914</v>
-      </c>
-      <c r="E267" t="s">
-        <v>979</v>
+        <v>979</v>
+      </c>
+      <c r="F267" t="s">
+        <v>642</v>
       </c>
       <c r="G267" t="s">
-        <v>926</v>
+        <v>920</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A268" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B268" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="C268" t="s">
         <v>642</v>
@@ -8175,12 +8187,18 @@
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A269" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B269" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C269" t="s">
+        <v>642</v>
+      </c>
+      <c r="D269" t="s">
+        <v>914</v>
+      </c>
+      <c r="E269" t="s">
         <v>979</v>
       </c>
       <c r="G269" t="s">
@@ -8189,10 +8207,10 @@
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A270" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B270" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C270" t="s">
         <v>979</v>
@@ -8203,84 +8221,72 @@
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A271" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B271" t="s">
-        <v>985</v>
+        <v>930</v>
       </c>
       <c r="C271" t="s">
-        <v>914</v>
-      </c>
-      <c r="D271" t="s">
-        <v>979</v>
-      </c>
-      <c r="E271" t="s">
-        <v>931</v>
+        <v>979</v>
       </c>
       <c r="G271" t="s">
-        <v>920</v>
+        <v>926</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A272" t="s">
-        <v>540</v>
+        <v>954</v>
       </c>
       <c r="B272" t="s">
-        <v>542</v>
+        <v>985</v>
+      </c>
+      <c r="C272" t="s">
+        <v>914</v>
       </c>
       <c r="D272" t="s">
-        <v>211</v>
+        <v>979</v>
+      </c>
+      <c r="E272" t="s">
+        <v>931</v>
       </c>
       <c r="G272" t="s">
-        <v>933</v>
+        <v>920</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A273" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B273" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D273" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G273" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A274" t="s">
-        <v>935</v>
+        <v>543</v>
       </c>
       <c r="B274" t="s">
-        <v>965</v>
-      </c>
-      <c r="C274" t="s">
-        <v>914</v>
+        <v>544</v>
       </c>
       <c r="D274" t="s">
-        <v>936</v>
-      </c>
-      <c r="E274" t="s">
-        <v>979</v>
-      </c>
-      <c r="F274" t="s">
-        <v>979</v>
+        <v>215</v>
       </c>
       <c r="G274" t="s">
-        <v>920</v>
-      </c>
-      <c r="H274" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A275" t="s">
-        <v>955</v>
+        <v>935</v>
       </c>
       <c r="B275" t="s">
-        <v>938</v>
+        <v>965</v>
       </c>
       <c r="C275" t="s">
         <v>914</v>
@@ -8297,33 +8303,39 @@
       <c r="G275" t="s">
         <v>920</v>
       </c>
+      <c r="H275" t="s">
+        <v>937</v>
+      </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A276" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B276" t="s">
-        <v>966</v>
+        <v>938</v>
       </c>
       <c r="C276" t="s">
-        <v>10</v>
+        <v>914</v>
       </c>
       <c r="D276" t="s">
-        <v>211</v>
+        <v>936</v>
+      </c>
+      <c r="E276" t="s">
+        <v>979</v>
       </c>
       <c r="F276" t="s">
-        <v>10</v>
+        <v>979</v>
       </c>
       <c r="G276" t="s">
-        <v>908</v>
+        <v>920</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A277" t="s">
-        <v>967</v>
+        <v>956</v>
       </c>
       <c r="B277" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="C277" t="s">
         <v>10</v>
@@ -8340,13 +8352,13 @@
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A278" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="B278" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="C278" t="s">
-        <v>914</v>
+        <v>10</v>
       </c>
       <c r="D278" t="s">
         <v>211</v>
@@ -8360,13 +8372,13 @@
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A279" t="s">
-        <v>977</v>
+        <v>969</v>
       </c>
       <c r="B279" t="s">
-        <v>978</v>
+        <v>970</v>
       </c>
       <c r="C279" t="s">
-        <v>10</v>
+        <v>914</v>
       </c>
       <c r="D279" t="s">
         <v>211</v>
@@ -8380,16 +8392,16 @@
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A280" t="s">
-        <v>971</v>
+        <v>977</v>
       </c>
       <c r="B280" t="s">
-        <v>972</v>
+        <v>978</v>
       </c>
       <c r="C280" t="s">
-        <v>914</v>
+        <v>10</v>
       </c>
       <c r="D280" t="s">
-        <v>936</v>
+        <v>211</v>
       </c>
       <c r="F280" t="s">
         <v>10</v>
@@ -8400,16 +8412,16 @@
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A281" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="B281" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="C281" t="s">
-        <v>10</v>
+        <v>914</v>
       </c>
       <c r="D281" t="s">
-        <v>211</v>
+        <v>936</v>
       </c>
       <c r="F281" t="s">
         <v>10</v>
@@ -8420,10 +8432,10 @@
     </row>
     <row r="282" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A282" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B282" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C282" t="s">
         <v>10</v>
@@ -8435,6 +8447,26 @@
         <v>10</v>
       </c>
       <c r="G282" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A283" t="s">
+        <v>974</v>
+      </c>
+      <c r="B283" t="s">
+        <v>976</v>
+      </c>
+      <c r="C283" t="s">
+        <v>10</v>
+      </c>
+      <c r="D283" t="s">
+        <v>211</v>
+      </c>
+      <c r="F283" t="s">
+        <v>10</v>
+      </c>
+      <c r="G283" t="s">
         <v>908</v>
       </c>
     </row>

</xml_diff>